<commit_message>
update 13 feb 2023
</commit_message>
<xml_diff>
--- a/Kas Hima - yrw - stthf.xlsx
+++ b/Kas Hima - yrw - stthf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03461a0c230c1ba6/Documents/Yofandi/rekap data - uang galon^J parkir^J bumbu asrama/uanghimastthf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{B3173F7A-21FF-40BD-9CB1-EB632A60ABC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52EA13C7-DF6D-427C-A5A1-56FADA13ACB4}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{B3173F7A-21FF-40BD-9CB1-EB632A60ABC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C624905-1CEF-4233-832F-8BB97EA51720}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="21792" windowHeight="12120" xr2:uid="{B1E7B7C2-6564-4E00-949B-823A851BA38E}"/>
   </bookViews>
@@ -79,6 +79,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,10 +120,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67E58695-AE7E-455B-A6CD-4D8C51602DBD}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,38 +459,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -523,13 +526,13 @@
       <c r="A9" s="1">
         <v>44930</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>365500</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>0</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <f>B9+C9</f>
         <v>365500</v>
       </c>
@@ -541,13 +544,13 @@
       <c r="A10" s="1">
         <v>44936</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>70000</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>0</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <f>D9+B10-C10</f>
         <v>435500</v>
       </c>
@@ -559,13 +562,13 @@
       <c r="A11" s="1">
         <v>44946</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>0</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>7500</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <f t="shared" ref="D11:D17" si="0">D10+B11-C11</f>
         <v>428000</v>
       </c>
@@ -577,13 +580,13 @@
       <c r="A12" s="1">
         <v>44958</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>65100</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>0</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="3">
         <f t="shared" si="0"/>
         <v>493100</v>
       </c>
@@ -595,13 +598,13 @@
       <c r="A13" s="1">
         <v>44967</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>10000</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <v>0</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <f t="shared" si="0"/>
         <v>503100</v>
       </c>
@@ -610,28 +613,66 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D14">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3">
         <f t="shared" si="0"/>
         <v>503100</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D15">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3">
         <f t="shared" si="0"/>
         <v>503100</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D16">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3">
         <f t="shared" si="0"/>
         <v>503100</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D17">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3">
         <f t="shared" si="0"/>
         <v>503100</v>
       </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D27" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
update 15 feb 2023
</commit_message>
<xml_diff>
--- a/Kas Hima - yrw - stthf.xlsx
+++ b/Kas Hima - yrw - stthf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03461a0c230c1ba6/Documents/Yofandi/rekap data - uang galon^J parkir^J bumbu asrama/uanghimastthf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{B3173F7A-21FF-40BD-9CB1-EB632A60ABC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C624905-1CEF-4233-832F-8BB97EA51720}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{B3173F7A-21FF-40BD-9CB1-EB632A60ABC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85B6E048-349F-43F1-841A-FE5E31CA27F8}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="21792" windowHeight="12120" xr2:uid="{B1E7B7C2-6564-4E00-949B-823A851BA38E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>*dimulai tanggal 14 Maret 2022</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>uang persembahan - intensif</t>
+  </si>
+  <si>
+    <t>pengeluaran belanja buat valentine</t>
+  </si>
+  <si>
+    <t>uang persembahan - reguler - valentine</t>
   </si>
 </sst>
 </file>
@@ -120,10 +126,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67E58695-AE7E-455B-A6CD-4D8C51602DBD}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,38 +465,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -526,13 +532,13 @@
       <c r="A9" s="1">
         <v>44930</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>365500</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>0</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <f>B9+C9</f>
         <v>365500</v>
       </c>
@@ -544,13 +550,13 @@
       <c r="A10" s="1">
         <v>44936</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>70000</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>0</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <f>D9+B10-C10</f>
         <v>435500</v>
       </c>
@@ -562,13 +568,13 @@
       <c r="A11" s="1">
         <v>44946</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>0</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>7500</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <f t="shared" ref="D11:D17" si="0">D10+B11-C11</f>
         <v>428000</v>
       </c>
@@ -580,13 +586,13 @@
       <c r="A12" s="1">
         <v>44958</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>65100</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>0</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>493100</v>
       </c>
@@ -598,13 +604,13 @@
       <c r="A13" s="1">
         <v>44967</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>10000</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>0</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>503100</v>
       </c>
@@ -613,66 +619,86 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3">
+      <c r="A14" s="1">
+        <v>44970</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>436000</v>
+      </c>
+      <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>503100</v>
+        <v>67100</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3">
+      <c r="A15" s="1">
+        <v>44972</v>
+      </c>
+      <c r="B15" s="2">
+        <v>95500</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>503100</v>
+        <v>162600</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>503100</v>
+        <v>162600</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2">
         <f t="shared" si="0"/>
-        <v>503100</v>
+        <v>162600</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D18" s="3"/>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D19" s="3"/>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D20" s="3"/>
+      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D21" s="3"/>
+      <c r="D21" s="2"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D22" s="3"/>
+      <c r="D22" s="2"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D23" s="3"/>
+      <c r="D23" s="2"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D24" s="3"/>
+      <c r="D24" s="2"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D25" s="3"/>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D26" s="3"/>
+      <c r="D26" s="2"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D27" s="3"/>
+      <c r="D27" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
update 26 apr 2023
</commit_message>
<xml_diff>
--- a/Kas Hima - yrw - stthf.xlsx
+++ b/Kas Hima - yrw - stthf.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03461a0c230c1ba6/Documents/Yofandi/rekap data - uang galon^J parkir^J bumbu asrama/uanghimastthf/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yofan\OneDrive\Documents\Yofandi\rekap data - uang galon, parkir, bumbu asrama\uanghimastthf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{8C076AFA-2F77-4570-9253-3C784C216761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE184B8-ABC2-48A3-8AE4-4D9B9A563BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="21792" windowHeight="12120" xr2:uid="{B1E7B7C2-6564-4E00-949B-823A851BA38E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
   <si>
     <t>*dimulai tanggal 14 Maret 2022</t>
   </si>
@@ -486,7 +486,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -816,38 +816,66 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C21" s="5"/>
+      <c r="A21" s="1">
+        <v>45037</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
+      <c r="C21" s="5">
+        <v>7500</v>
+      </c>
       <c r="D21" s="2">
         <f t="shared" si="0"/>
-        <v>426400</v>
+        <v>418900</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C22" s="5"/>
+      <c r="A22" s="1">
+        <v>45042</v>
+      </c>
+      <c r="B22" s="2">
+        <v>32000</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0</v>
+      </c>
       <c r="D22" s="2">
         <f t="shared" si="0"/>
-        <v>426400</v>
+        <v>450900</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C23" s="5"/>
       <c r="D23" s="2">
         <f t="shared" si="0"/>
-        <v>426400</v>
+        <v>450900</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C24" s="5"/>
       <c r="D24" s="2">
         <f t="shared" si="0"/>
-        <v>426400</v>
+        <v>450900</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C25" s="5"/>
       <c r="D25" s="2">
         <f t="shared" si="0"/>
-        <v>426400</v>
+        <v>450900</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update 17 mei 2023
</commit_message>
<xml_diff>
--- a/Kas Hima - yrw - stthf.xlsx
+++ b/Kas Hima - yrw - stthf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yofan\OneDrive\Documents\Yofandi\rekap data - uang galon, parkir, bumbu asrama\uanghimastthf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03461a0c230c1ba6/Documents/Yofandi/rekap data - uang galon^J parkir^J bumbu asrama/uanghimastthf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE184B8-ABC2-48A3-8AE4-4D9B9A563BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{6CE184B8-ABC2-48A3-8AE4-4D9B9A563BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAFBC37F-A45C-4F18-B5E5-914581C524D3}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="21792" windowHeight="12120" xr2:uid="{B1E7B7C2-6564-4E00-949B-823A851BA38E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B1E7B7C2-6564-4E00-949B-823A851BA38E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
   <si>
     <t>*dimulai tanggal 14 Maret 2022</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>uang persembahan</t>
+  </si>
+  <si>
+    <t>uang santunan dukacita untuk keluargag kak safe</t>
   </si>
 </sst>
 </file>
@@ -184,6 +187,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -485,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67E58695-AE7E-455B-A6CD-4D8C51602DBD}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -858,24 +865,52 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C23" s="5"/>
+      <c r="A23" s="1">
+        <v>45057</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0</v>
+      </c>
+      <c r="C23" s="5">
+        <v>200000</v>
+      </c>
       <c r="D23" s="2">
         <f t="shared" si="0"/>
-        <v>450900</v>
+        <v>250900</v>
+      </c>
+      <c r="E23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C24" s="5"/>
+      <c r="A24" s="1">
+        <v>45063</v>
+      </c>
+      <c r="B24" s="2">
+        <v>70000</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0</v>
+      </c>
       <c r="D24" s="2">
         <f t="shared" si="0"/>
-        <v>450900</v>
+        <v>320900</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C25" s="5"/>
       <c r="D25" s="2">
         <f t="shared" si="0"/>
-        <v>450900</v>
+        <v>320900</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update 08 juni 2023
</commit_message>
<xml_diff>
--- a/Kas Hima - yrw - stthf.xlsx
+++ b/Kas Hima - yrw - stthf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03461a0c230c1ba6/Documents/Yofandi/rekap data - uang galon^J parkir^J bumbu asrama/uanghimastthf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{6CE184B8-ABC2-48A3-8AE4-4D9B9A563BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAFBC37F-A45C-4F18-B5E5-914581C524D3}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{6CE184B8-ABC2-48A3-8AE4-4D9B9A563BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C6B5CDA-E585-427C-B758-B3D3C3875F8C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B1E7B7C2-6564-4E00-949B-823A851BA38E}"/>
+    <workbookView xWindow="1116" yWindow="840" windowWidth="21792" windowHeight="12120" xr2:uid="{B1E7B7C2-6564-4E00-949B-823A851BA38E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t>*dimulai tanggal 14 Maret 2022</t>
   </si>
@@ -187,10 +187,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -492,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67E58695-AE7E-455B-A6CD-4D8C51602DBD}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -907,10 +903,24 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C25" s="5"/>
+      <c r="A25" s="1">
+        <v>45083</v>
+      </c>
+      <c r="B25" s="2">
+        <v>39000</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0</v>
+      </c>
       <c r="D25" s="2">
         <f t="shared" si="0"/>
-        <v>320900</v>
+        <v>359900</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update 22 agustus 2023
</commit_message>
<xml_diff>
--- a/Kas Hima - yrw - stthf.xlsx
+++ b/Kas Hima - yrw - stthf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03461a0c230c1ba6/Documents/Yofandi/rekap data - uang galon^J parkir^J bumbu asrama/uanghimastthf/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03461a0c230c1ba6/Documents/Yofandi/Kuliah STT Happy Familiy/rekap data - uang galon^J parkir^J bumbu asrama/uanghimastthf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{6CE184B8-ABC2-48A3-8AE4-4D9B9A563BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C6B5CDA-E585-427C-B758-B3D3C3875F8C}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{6CE184B8-ABC2-48A3-8AE4-4D9B9A563BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7ABE480E-6B43-4667-9D42-031FFA74C21F}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="840" windowWidth="21792" windowHeight="12120" xr2:uid="{B1E7B7C2-6564-4E00-949B-823A851BA38E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B1E7B7C2-6564-4E00-949B-823A851BA38E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="20">
   <si>
     <t>*dimulai tanggal 14 Maret 2022</t>
   </si>
@@ -486,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67E58695-AE7E-455B-A6CD-4D8C51602DBD}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,7 +619,7 @@
         <v>7500</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" ref="D11:D25" si="0">D10+B11-C11</f>
+        <f t="shared" ref="D11:D32" si="0">D10+B11-C11</f>
         <v>428000</v>
       </c>
       <c r="E11" t="s">
@@ -904,53 +904,177 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
+        <v>45074</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0</v>
+      </c>
+      <c r="C25" s="5">
+        <v>7500</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="0"/>
+        <v>313400</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
         <v>45083</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B26" s="2">
         <v>39000</v>
       </c>
-      <c r="C25" s="5">
-        <v>0</v>
-      </c>
-      <c r="D25" s="2">
-        <f t="shared" si="0"/>
-        <v>359900</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="C26" s="5">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="0"/>
+        <v>352400</v>
+      </c>
+      <c r="E26" t="s">
         <v>10</v>
       </c>
-      <c r="F25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C26" s="5"/>
-      <c r="D26" s="2"/>
+      <c r="F26" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C27" s="5"/>
-      <c r="D27" s="2"/>
+      <c r="A27" s="1">
+        <v>45093</v>
+      </c>
+      <c r="C27" s="5">
+        <v>7500</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" si="0"/>
+        <v>344900</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C28" s="5"/>
+      <c r="A28" s="1">
+        <v>45096</v>
+      </c>
+      <c r="B28" s="2">
+        <v>73000</v>
+      </c>
+      <c r="C28" s="5">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="0"/>
+        <v>417900</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C29" s="5"/>
+      <c r="A29" s="1">
+        <v>45110</v>
+      </c>
+      <c r="B29" s="2">
+        <v>30000</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="0"/>
+        <v>447900</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C30" s="5"/>
+      <c r="A30" s="1">
+        <v>45124</v>
+      </c>
+      <c r="B30" s="2">
+        <v>30000</v>
+      </c>
+      <c r="C30" s="5">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="0"/>
+        <v>477900</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C31" s="5"/>
+      <c r="A31" s="1">
+        <v>45129</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0</v>
+      </c>
+      <c r="C31" s="5">
+        <v>7500</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="0"/>
+        <v>470400</v>
+      </c>
+      <c r="E31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="5"/>
+      <c r="A32" s="1">
+        <v>45156</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0</v>
+      </c>
+      <c r="C32" s="5">
+        <v>7500</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" si="0"/>
+        <v>462900</v>
+      </c>
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" s="5"/>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C34" s="5"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C35" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>